<commit_message>
jeux de données id
</commit_message>
<xml_diff>
--- a/src/metriques cas initial/Copie de gabarit_jeux_essais_ID_Classes.xlsx
+++ b/src/metriques cas initial/Copie de gabarit_jeux_essais_ID_Classes.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="gabarit jeux" sheetId="2" r:id="rId1"/>
+    <sheet name="jeux de données id" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>Jeux d'essais</t>
   </si>
@@ -65,14 +66,200 @@
     <t>TP2_1</t>
   </si>
   <si>
-    <t>Note: Le même jeux d'essais pour toutes les classes, comme titre d'example on a pris la classe Employe</t>
+    <t>Employe</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t>setId</t>
+  </si>
+  <si>
+    <t>Réussi</t>
+  </si>
+  <si>
+    <t>em2016aa11</t>
+  </si>
+  <si>
+    <t>Jeu d'essai valide</t>
+  </si>
+  <si>
+    <t>Jeu d'essai avec caractères spéciaux</t>
+  </si>
+  <si>
+    <t>Échec</t>
+  </si>
+  <si>
+    <t>em2016@a11</t>
+  </si>
+  <si>
+    <t>Jeu d'essai avec espaces après</t>
+  </si>
+  <si>
+    <t>em2016aa1</t>
+  </si>
+  <si>
+    <t>Jeu d'essai avec espace comme séparateur ou  milieux</t>
+  </si>
+  <si>
+    <t>em2016 a11</t>
+  </si>
+  <si>
+    <t>Jeu d'essai vide</t>
+  </si>
+  <si>
+    <t>ed2016aa11</t>
+  </si>
+  <si>
+    <t>Jeu d'essai avec la deuxieme lettre different de celle de la classe</t>
+  </si>
+  <si>
+    <t>Jeu d'essai qui ne contient pas l'année courante</t>
+  </si>
+  <si>
+    <t>em2015aa11</t>
+  </si>
+  <si>
+    <t>em2016</t>
+  </si>
+  <si>
+    <t>Jeu d'essai qui a une longueur plus petite que 10 caractères</t>
+  </si>
+  <si>
+    <t>Jeu d'essai qui a une longueur plus grand que 10 caractères</t>
+  </si>
+  <si>
+    <t>em2016aa1122</t>
+  </si>
+  <si>
+    <t>TP2_2</t>
+  </si>
+  <si>
+    <t>TP2_3</t>
+  </si>
+  <si>
+    <t>TP2_4</t>
+  </si>
+  <si>
+    <t>TP2_5</t>
+  </si>
+  <si>
+    <t>TP2_6</t>
+  </si>
+  <si>
+    <t>TP2_7</t>
+  </si>
+  <si>
+    <t>TP2_8</t>
+  </si>
+  <si>
+    <t>TP2_9</t>
+  </si>
+  <si>
+    <t>Sous-Domaine</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Exemple</t>
+  </si>
+  <si>
+    <t>Résultat</t>
+  </si>
+  <si>
+    <t>Longueur identifiant</t>
+  </si>
+  <si>
+    <t>longueur de 10 caractères</t>
+  </si>
+  <si>
+    <t>longueur de 6 caractères</t>
+  </si>
+  <si>
+    <t>échec</t>
+  </si>
+  <si>
+    <t>ne contient que des espaces vides</t>
+  </si>
+  <si>
+    <t>espaces blancs</t>
+  </si>
+  <si>
+    <t>rien n'est entré</t>
+  </si>
+  <si>
+    <t>vide</t>
+  </si>
+  <si>
+    <t>succès</t>
+  </si>
+  <si>
+    <t>longueur de 12 caractères</t>
+  </si>
+  <si>
+    <t>longueur de 8 caractères</t>
+  </si>
+  <si>
+    <t>em2016aa</t>
+  </si>
+  <si>
+    <t>les caractères 3-6 représentent l'année courant</t>
+  </si>
+  <si>
+    <t>ne continet pas l'année</t>
+  </si>
+  <si>
+    <t>emaaff11vv</t>
+  </si>
+  <si>
+    <t>Chiffre</t>
+  </si>
+  <si>
+    <t>contient l'année courant</t>
+  </si>
+  <si>
+    <t>l'année n'est pas valide</t>
+  </si>
+  <si>
+    <t>Lettres</t>
+  </si>
+  <si>
+    <t>contenant les 2 premiere lettres de la classe</t>
+  </si>
+  <si>
+    <t>ne commence pas avec les 2 premieres lettres de la classe(example classe Employe)</t>
+  </si>
+  <si>
+    <t>bb2016aa11</t>
+  </si>
+  <si>
+    <t>ne commence pas avec des lettres</t>
+  </si>
+  <si>
+    <t>2016aa11bb</t>
+  </si>
+  <si>
+    <t>commence avec les 2 premieres lettres de la classe(example classe Employe)</t>
+  </si>
+  <si>
+    <t>Caractère spécial</t>
+  </si>
+  <si>
+    <t>contient des caractères alphabétiques</t>
+  </si>
+  <si>
+    <t>ne contient aucun caractère spécial</t>
+  </si>
+  <si>
+    <t>contient 1 caractère spécial</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,8 +275,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,8 +303,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -126,11 +339,284 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -159,14 +645,94 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -473,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:I17"/>
+  <dimension ref="C6:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -486,7 +1052,7 @@
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="23" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="8" max="8" width="58.5703125" customWidth="1"/>
     <col min="9" max="9" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -516,7 +1082,9 @@
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="9"/>
+      <c r="D8" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -527,14 +1095,14 @@
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="10">
         <v>42492</v>
       </c>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
@@ -572,43 +1140,178 @@
       <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="F12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
+      <c r="C13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="C14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="C15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>12</v>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="2"/>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C19" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2"/>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -619,7 +1322,299 @@
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="D10:I10"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F20" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C6:G25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="5" max="5" width="78.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="24"/>
+      <c r="D9" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="24"/>
+      <c r="D10" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="24"/>
+      <c r="D11" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="24"/>
+      <c r="D12" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F12" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="24"/>
+      <c r="D13" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="F13" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="28"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="50"/>
+    </row>
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="24"/>
+      <c r="D15" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F16" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="24"/>
+      <c r="D17" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="50"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="24"/>
+      <c r="D20" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="24"/>
+      <c r="D21" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22" s="34"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="37"/>
+      <c r="G22" s="38"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C23" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="43" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C24" s="39"/>
+      <c r="D24" s="40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="45"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="49"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C7:D7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F24" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>